<commit_message>
July 22, 2021 update
- Updated German states and country data
</commit_message>
<xml_diff>
--- a/static/data/GermanyAllNumbersXLSX.xlsx
+++ b/static/data/GermanyAllNumbersXLSX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nancyyu/Documents/R website/First_Website/static/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598B9AAB-D533-854E-B94B-C07FF4B57BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF139C33-093A-CD49-909F-4FCA4F24882E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32500" yWindow="500" windowWidth="27980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="500" windowWidth="28020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GermanyAllNumbers" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="44">
   <si>
     <t>iso_code</t>
   </si>
@@ -1014,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX494"/>
+  <dimension ref="A1:AX496"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A461" workbookViewId="0">
-      <selection activeCell="H495" sqref="H495"/>
+      <selection activeCell="H497" sqref="H497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39032,7 +39032,7 @@
         <v>42</v>
       </c>
       <c r="D478" s="1">
-        <f t="shared" ref="D478:D494" si="665">D477+1</f>
+        <f t="shared" ref="D478:D496" si="665">D477+1</f>
         <v>44381</v>
       </c>
       <c r="E478">
@@ -39914,7 +39914,7 @@
         <v>44397</v>
       </c>
       <c r="E494">
-        <f t="shared" ref="E492:E494" si="677">E493+F494</f>
+        <f t="shared" ref="E494" si="677">E493+F494</f>
         <v>3746410</v>
       </c>
       <c r="F494" s="4">
@@ -39951,6 +39951,116 @@
         <v>0</v>
       </c>
       <c r="P494" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A495" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B495" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C495" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D495" s="1">
+        <f t="shared" si="665"/>
+        <v>44398</v>
+      </c>
+      <c r="E495">
+        <f t="shared" ref="E495" si="678">E494+F495</f>
+        <v>3748613</v>
+      </c>
+      <c r="F495" s="4">
+        <v>2203</v>
+      </c>
+      <c r="G495" s="2">
+        <f t="shared" ref="G495" si="679">SUM(F489:F495)/7</f>
+        <v>1418.5714285714287</v>
+      </c>
+      <c r="H495" s="4">
+        <v>91416</v>
+      </c>
+      <c r="I495">
+        <f t="shared" ref="I495" si="680">H495-H494</f>
+        <v>19</v>
+      </c>
+      <c r="J495" s="2">
+        <f t="shared" ref="J495" si="681">SUM(I489:I495)/7</f>
+        <v>18.428571428571427</v>
+      </c>
+      <c r="K495" s="4">
+        <v>0</v>
+      </c>
+      <c r="L495" s="4">
+        <v>0</v>
+      </c>
+      <c r="M495" s="4">
+        <v>0</v>
+      </c>
+      <c r="N495" s="4">
+        <v>0</v>
+      </c>
+      <c r="O495" s="4">
+        <v>0</v>
+      </c>
+      <c r="P495" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A496" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B496" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C496" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D496" s="1">
+        <f t="shared" si="665"/>
+        <v>44399</v>
+      </c>
+      <c r="E496">
+        <f t="shared" ref="E496" si="682">E495+F496</f>
+        <v>3750503</v>
+      </c>
+      <c r="F496" s="4">
+        <v>1890</v>
+      </c>
+      <c r="G496" s="2">
+        <f t="shared" ref="G496" si="683">SUM(F490:F496)/7</f>
+        <v>1454</v>
+      </c>
+      <c r="H496" s="4">
+        <v>91458</v>
+      </c>
+      <c r="I496">
+        <f t="shared" ref="I496" si="684">H496-H495</f>
+        <v>42</v>
+      </c>
+      <c r="J496" s="2">
+        <f t="shared" ref="J496" si="685">SUM(I490:I496)/7</f>
+        <v>19.857142857142858</v>
+      </c>
+      <c r="K496" s="4">
+        <v>0</v>
+      </c>
+      <c r="L496" s="4">
+        <v>0</v>
+      </c>
+      <c r="M496" s="4">
+        <v>0</v>
+      </c>
+      <c r="N496" s="4">
+        <v>0</v>
+      </c>
+      <c r="O496" s="4">
+        <v>0</v>
+      </c>
+      <c r="P496" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>